<commit_message>
Digikey broke my heart, changed from html to json
</commit_message>
<xml_diff>
--- a/aqs_bot/parts_sourcing/input/component_library.xlsx
+++ b/aqs_bot/parts_sourcing/input/component_library.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Izzat Khair\Desktop\School\Y3T1\FYP\public_code\fyp\aqs_bot\parts_sourcing\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150B2326-7277-4514-8A83-4DE73DDA5719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD3FC46-7345-4768-9D35-C3BF6884FE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Component number</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Z513A0302511</t>
+  </si>
+  <si>
+    <t>L34A196</t>
+  </si>
+  <si>
+    <t>2002-1492</t>
   </si>
 </sst>
 </file>
@@ -444,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -575,6 +581,24 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>